<commit_message>
Header updated, added TLS header
</commit_message>
<xml_diff>
--- a/samples/sampleOSSPullInput.xlsx
+++ b/samples/sampleOSSPullInput.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohadisraeli/Documents/Redis/CloudClusterInfo/EC2RL-Internal/samples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/5nip3r/Development/GIT/ecstats/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057B2CB2-2FB9-3744-AD29-132442A289E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320C2387-0FDE-3F4D-90C5-4AE3400A0394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>DB Name</t>
   </si>
@@ -37,29 +37,32 @@
     <t>User (ACL)</t>
   </si>
   <si>
-    <t>Demo</t>
-  </si>
-  <si>
-    <t>demo.com</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>pwd</t>
+    <t>TLS</t>
+  </si>
+  <si>
+    <t>demo</t>
+  </si>
+  <si>
+    <t>192.168.29.50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF323130"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -82,8 +85,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,23 +426,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,28 +454,28 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>12000</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
+        <v>6379</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>